<commit_message>
COMMON - add logger
</commit_message>
<xml_diff>
--- a/DetailInfo/TTO_PROJECT_DESIGN.xlsx
+++ b/DetailInfo/TTO_PROJECT_DESIGN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1039,17 +1039,8 @@
   </cellStyleXfs>
   <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1059,18 +1050,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,23 +1112,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1157,25 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1190,29 +1139,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1224,6 +1152,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1236,15 +1194,57 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2020,7 +2020,8 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="31750">
-          <a:tailEnd type="arrow"/>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2216,6 +2217,329 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="圆角矩形 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1447800" y="3076575"/>
+          <a:ext cx="1695450" cy="942975"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="T0" fmla="*/ 46032 w 1695450"/>
+            <a:gd name="T1" fmla="*/ 46032 h 942975"/>
+            <a:gd name="T2" fmla="*/ 1649417 w 1695450"/>
+            <a:gd name="T3" fmla="*/ 896942 h 942975"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="0" y="157165"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="0" y="157165"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="157164" y="0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="1538284" y="0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="1538283" y="0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="1695449" y="157165"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="1695450" y="785809"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="1695450" y="785809"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="1538285" y="942974"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="157165" y="942975"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="157165" y="942975"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="0" y="785810"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="1695450" h="942975">
+              <a:moveTo>
+                <a:pt x="0" y="157165"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="157165"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="0" y="70365"/>
+                <a:pt x="70365" y="0"/>
+                <a:pt x="157164" y="0"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1538284" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1538283" y="0"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1625083" y="0"/>
+                <a:pt x="1695449" y="70365"/>
+                <a:pt x="1695449" y="157165"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1695450" y="785809"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1695450" y="872608"/>
+                <a:pt x="1625084" y="942973"/>
+                <a:pt x="1538285" y="942974"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="157165" y="942975"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="70365" y="942975"/>
+                <a:pt x="0" y="872609"/>
+                <a:pt x="0" y="785810"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000"/>
+        </a:gradFill>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="宋体"/>
+              <a:ea typeface="宋体"/>
+            </a:rPr>
+            <a:t>TTO_Auto_Task</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="2266950"/>
+          <a:ext cx="4114800" cy="2038350"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextBox 25"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247775" y="2428875"/>
+          <a:ext cx="2447925" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>TTO_Admin</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Elbow Connector 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="3076" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2200276" y="4000502"/>
+          <a:ext cx="3457574" cy="2024061"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -138"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln w="31750">
           <a:tailEnd type="arrow"/>
@@ -6421,186 +6745,186 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="7" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="7" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="18.75">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="10" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6641,147 +6965,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="30">
+      <c r="A11" s="23">
         <v>42239</v>
       </c>
       <c r="B11" t="s">
@@ -6789,7 +7113,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="30">
+      <c r="A12" s="23">
         <v>42240</v>
       </c>
       <c r="B12" t="s">
@@ -6797,7 +7121,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="30">
+      <c r="A13" s="23">
         <v>42241</v>
       </c>
       <c r="B13" t="s">
@@ -6805,7 +7129,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="30">
+      <c r="A14" s="23">
         <v>42242</v>
       </c>
       <c r="B14" t="s">
@@ -6813,7 +7137,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="30">
+      <c r="A15" s="23">
         <v>42243</v>
       </c>
       <c r="B15" t="s">
@@ -6821,7 +7145,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="30">
+      <c r="A16" s="23">
         <v>42244</v>
       </c>
       <c r="B16" t="s">
@@ -6852,593 +7176,598 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="64"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="66"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="56"/>
+      <c r="B3" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="64"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="54"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="66"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="63" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="64"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="67"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="63" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="64"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="54"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="70" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="38"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="39" t="s">
+      <c r="A7" s="68"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="38"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="39" t="s">
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="63"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="38"/>
-      <c r="B9" s="42" t="s">
+      <c r="A9" s="68"/>
+      <c r="B9" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="38"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="39" t="s">
+      <c r="A10" s="68"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="39" t="s">
+      <c r="A11" s="68"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="63"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44" t="s">
+      <c r="A12" s="68"/>
+      <c r="B12" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="63"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="38"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="39" t="s">
+      <c r="A13" s="68"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="63"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="38"/>
-      <c r="B14" s="46" t="s">
+      <c r="A14" s="68"/>
+      <c r="B14" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="63"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="37" t="s">
+      <c r="E15" s="29"/>
+      <c r="F15" s="70" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="47"/>
-      <c r="B16" s="51" t="s">
+      <c r="A16" s="72"/>
+      <c r="B16" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="63"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="47"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="72"/>
+      <c r="B17" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="63"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="47"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="50" t="s">
+      <c r="A18" s="72"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="63"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="47"/>
-      <c r="B19" s="43" t="s">
+      <c r="A19" s="72"/>
+      <c r="B19" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="63"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="47"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="50" t="s">
+      <c r="A20" s="72"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="63"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="47"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="72"/>
+      <c r="B21" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="63"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="47"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="50" t="s">
+      <c r="A22" s="72"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="41"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="63"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="47"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="50" t="s">
+      <c r="A23" s="72"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="63"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="53"/>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="73"/>
+      <c r="B24" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="63"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="53"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="54" t="s">
+      <c r="A25" s="73"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="63"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="53"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="73"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="63"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="47"/>
-      <c r="B27" s="42" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="41"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="63"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="55"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="50" t="s">
+      <c r="A28" s="60"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="56"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="64"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41" t="s">
+      <c r="E29" s="29"/>
+      <c r="F29" s="63" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="57"/>
-      <c r="B30" s="43" t="s">
+      <c r="A30" s="61"/>
+      <c r="B30" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="63"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="57"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="50" t="s">
+      <c r="A31" s="61"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="41"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="63"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="57"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="50" t="s">
+      <c r="A32" s="61"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="41"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="63"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="57"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="50" t="s">
+      <c r="A33" s="61"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="63"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="57"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="50" t="s">
+      <c r="A34" s="61"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="63"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="57"/>
-      <c r="B35" s="43" t="s">
+      <c r="A35" s="61"/>
+      <c r="B35" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="63"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="57"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="50" t="s">
+      <c r="A36" s="61"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="63"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="57"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="50" t="s">
+      <c r="A37" s="61"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="63"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="57"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="50" t="s">
+      <c r="A38" s="61"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="41"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="63"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="57"/>
-      <c r="B39" s="43" t="s">
+      <c r="A39" s="61"/>
+      <c r="B39" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="63"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="57"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="50" t="s">
+      <c r="A40" s="61"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="63"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="57"/>
-      <c r="B41" s="43" t="s">
+      <c r="A41" s="61"/>
+      <c r="B41" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="41"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="63"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="57"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="50" t="s">
+      <c r="A42" s="61"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="41"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="63"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="57"/>
-      <c r="B43" s="8" t="s">
+      <c r="A43" s="61"/>
+      <c r="B43" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="41"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="63"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="58"/>
-      <c r="B44" s="59"/>
-      <c r="C44" s="60" t="s">
+      <c r="A44" s="62"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="61"/>
-      <c r="F44" s="56"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A15:A28"/>
+    <mergeCell ref="F15:F28"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B23"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B24:B26"/>
@@ -7455,11 +7784,6 @@
     <mergeCell ref="F6:F14"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A15:A28"/>
-    <mergeCell ref="F15:F28"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7469,8 +7793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7491,624 +7815,624 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="69" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8127,10 +8451,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="9" spans="18:18">
-      <c r="R9" s="70"/>
+      <c r="R9" s="42"/>
     </row>
     <row r="27" spans="15:15">
-      <c r="O27" s="70"/>
+      <c r="O27" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8158,397 +8482,397 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="E2" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="71" t="s">
+      <c r="G2" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="43" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="3:9">
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="44" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="4" spans="3:9">
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="E4" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="45" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="5" spans="3:9">
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="I5" s="73" t="s">
+      <c r="I5" s="45" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="6" spans="3:9">
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="45" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="7" spans="3:9">
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="71" t="s">
+      <c r="E7" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="74" t="s">
+      <c r="G7" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="73" t="s">
+      <c r="I7" s="45" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="3:9">
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="I8" s="45" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="9" spans="3:9">
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="I9" s="73" t="s">
+      <c r="I9" s="45" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="10" spans="3:9">
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="45" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" spans="3:9">
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="G11" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="I11" s="73" t="s">
+      <c r="I11" s="45" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="12" spans="3:9">
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="E12" s="71" t="s">
+      <c r="E12" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="G12" s="73" t="s">
+      <c r="G12" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="I12" s="74" t="s">
+      <c r="I12" s="46" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="13" spans="3:9">
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="45" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="14" spans="3:9">
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="E14" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="G14" s="73" t="s">
+      <c r="G14" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="I14" s="71" t="s">
+      <c r="I14" s="43" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="15" spans="3:9">
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="I15" s="72" t="s">
+      <c r="I15" s="44" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="16" spans="3:9">
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="73" t="s">
+      <c r="E16" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="73" t="s">
+      <c r="G16" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="45" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="17" spans="3:9">
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="G17" s="73" t="s">
+      <c r="G17" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="I17" s="74" t="s">
+      <c r="I17" s="46" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="18" spans="3:9">
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="G18" s="45" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="19" spans="3:9">
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="I19" s="71" t="s">
+      <c r="I19" s="43" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="3:9">
-      <c r="E20" s="71" t="s">
+      <c r="E20" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G20" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="72" t="s">
+      <c r="I20" s="44" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="21" spans="3:9">
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="72" t="s">
+      <c r="E21" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G21" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="I21" s="73" t="s">
+      <c r="I21" s="45" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="22" spans="3:9">
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="73" t="s">
+      <c r="E22" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="G22" s="73" t="s">
+      <c r="G22" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="I22" s="73" t="s">
+      <c r="I22" s="45" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="23" spans="3:9">
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="E23" s="73" t="s">
+      <c r="E23" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="G23" s="73" t="s">
+      <c r="G23" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="I23" s="73" t="s">
+      <c r="I23" s="45" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="24" spans="3:9">
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="E24" s="74" t="s">
+      <c r="E24" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="G24" s="73" t="s">
+      <c r="G24" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="I24" s="73" t="s">
+      <c r="I24" s="45" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="25" spans="3:9">
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="G25" s="73" t="s">
+      <c r="G25" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="I25" s="73" t="s">
+      <c r="I25" s="45" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="26" spans="3:9">
-      <c r="E26" s="71" t="s">
+      <c r="E26" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="G26" s="73" t="s">
+      <c r="G26" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="I26" s="73" t="s">
+      <c r="I26" s="45" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="27" spans="3:9">
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="G27" s="73" t="s">
+      <c r="G27" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="I27" s="73" t="s">
+      <c r="I27" s="45" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="28" spans="3:9">
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="G28" s="73" t="s">
+      <c r="G28" s="45" t="s">
         <v>208</v>
       </c>
-      <c r="I28" s="73" t="s">
+      <c r="I28" s="45" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="29" spans="3:9">
-      <c r="E29" s="73" t="s">
+      <c r="E29" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="G29" s="73" t="s">
+      <c r="G29" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="I29" s="73" t="s">
+      <c r="I29" s="45" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="30" spans="3:9">
-      <c r="E30" s="73" t="s">
+      <c r="E30" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="G30" s="73" t="s">
+      <c r="G30" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I30" s="73" t="s">
+      <c r="I30" s="45" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="3:9">
-      <c r="E31" s="73" t="s">
+      <c r="E31" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="G31" s="74" t="s">
+      <c r="G31" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="I31" s="73" t="s">
+      <c r="I31" s="45" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="32" spans="3:9">
-      <c r="E32" s="73" t="s">
+      <c r="E32" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="I32" s="73" t="s">
+      <c r="I32" s="45" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="33" spans="5:9">
-      <c r="E33" s="73" t="s">
+      <c r="E33" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I33" s="73" t="s">
+      <c r="I33" s="45" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="34" spans="5:9">
-      <c r="E34" s="74" t="s">
+      <c r="E34" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="73" t="s">
+      <c r="I34" s="45" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="35" spans="5:9">
-      <c r="I35" s="74" t="s">
+      <c r="I35" s="46" t="s">
         <v>144</v>
       </c>
     </row>
@@ -8562,7 +8886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>

</xml_diff>